<commit_message>
popravila tabele za nike in adidas
</commit_message>
<xml_diff>
--- a/Data-Adidas/Bilanca_adidas.xlsx
+++ b/Data-Adidas/Bilanca_adidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Exchange rate: EUR/USD</t>
   </si>
@@ -35,30 +35,9 @@
     <t>Fixed assets</t>
   </si>
   <si>
-    <t xml:space="preserve"> ∟ Intangible fixed assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Tangible fixed assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Other fixed assets</t>
-  </si>
-  <si>
     <t>Current assets</t>
   </si>
   <si>
-    <t xml:space="preserve"> ∟ Stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Debtors</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Other current assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Cash &amp; cash equivalent</t>
-  </si>
-  <si>
     <t>Total assets</t>
   </si>
   <si>
@@ -68,52 +47,58 @@
     <t>Shareholders funds</t>
   </si>
   <si>
-    <t xml:space="preserve"> ∟ Capital</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Other shareholders funds</t>
-  </si>
-  <si>
     <t>Non-current liabilities</t>
   </si>
   <si>
-    <t xml:space="preserve"> ∟ Long term debt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Other non-current liabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Provisions</t>
-  </si>
-  <si>
     <t>Current liabilities</t>
   </si>
   <si>
-    <t xml:space="preserve"> ∟ Loans</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Creditors</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Other current liabilities</t>
-  </si>
-  <si>
     <t>Total shareh. funds &amp; liab.</t>
   </si>
   <si>
-    <t>Memo lines</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Working capital</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Net current assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Enterprise value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ∟ Number of employees</t>
+    <t>Intangible fixed assets</t>
+  </si>
+  <si>
+    <t>Tangible fixed assets</t>
+  </si>
+  <si>
+    <t>Other fixed assets</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Debtors</t>
+  </si>
+  <si>
+    <t>Other current assets</t>
+  </si>
+  <si>
+    <t>Cash &amp; cash equivalent</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>Other shareholders funds</t>
+  </si>
+  <si>
+    <t>Long term debt</t>
+  </si>
+  <si>
+    <t>Other non-current liabilities</t>
+  </si>
+  <si>
+    <t>Provisions</t>
+  </si>
+  <si>
+    <t>Loans</t>
+  </si>
+  <si>
+    <t>Creditors</t>
+  </si>
+  <si>
+    <t>Other current liabilities</t>
   </si>
 </sst>
 </file>
@@ -121,9 +106,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="170" formatCode="###,##0"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="166" formatCode="###,##0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -218,32 +203,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -527,18 +522,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3">
         <v>43830</v>
@@ -552,8 +548,11 @@
       <c r="E1" s="3">
         <v>42735</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F1" s="11">
+        <v>42369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -569,8 +568,11 @@
       <c r="E2" s="5">
         <v>1.0541</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="12">
+        <v>1.0887</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -578,8 +580,9 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -595,10 +598,13 @@
       <c r="E4" s="7">
         <v>6630286.2310409499</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="F4" s="13">
+        <v>6364539.8309230804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" s="7">
         <v>2719751.0458231</v>
@@ -612,10 +618,13 @@
       <c r="E5" s="7">
         <v>3435310.4653358501</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="F5" s="13">
+        <v>3492549.3974685702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" s="7">
         <v>2673691.6518211402</v>
@@ -629,10 +638,13 @@
       <c r="E6" s="7">
         <v>2018600.6569862401</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F6" s="13">
+        <v>1783290.49658775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>5555212.2765779505</v>
@@ -646,10 +658,13 @@
       <c r="E7" s="7">
         <v>1176375.10871887</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F7" s="13">
+        <v>1088699.93686676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="7">
         <v>12283254.0004253</v>
@@ -663,10 +678,13 @@
       <c r="E8" s="7">
         <v>9366728.6882400494</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="13">
+        <v>8161983.4266900998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B9" s="7">
         <v>4589088.40239048</v>
@@ -680,10 +698,13 @@
       <c r="E9" s="7">
         <v>3966576.6434669499</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F9" s="13">
+        <v>3389122.90346622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B10" s="7">
         <v>2948924.61597919</v>
@@ -697,10 +718,13 @@
       <c r="E10" s="7">
         <v>2319019.0315246601</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F10" s="13">
+        <v>2230746.1706399899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11" s="7">
         <v>4745240.9820556603</v>
@@ -714,10 +738,13 @@
       <c r="E11" s="7">
         <v>3081133.0132484399</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F11" s="13">
+        <v>2542114.3525838898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12" s="7">
         <v>2821980.4325103802</v>
@@ -731,10 +758,13 @@
       <c r="E12" s="7">
         <v>1677072.3996162401</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="13">
+        <v>1486075.4138231301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B13" s="9">
         <v>23231908.9746475</v>
@@ -748,19 +778,23 @@
       <c r="E13" s="9">
         <v>15997014.919281</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="14">
+        <v>14526523.257613201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B15" s="7">
         <v>7928956.1674594898</v>
@@ -774,10 +808,13 @@
       <c r="E15" s="7">
         <v>6804212.6584053002</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F15" s="13">
+        <v>6148977.2434234601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7">
         <v>220186.371326447</v>
@@ -791,10 +828,13 @@
       <c r="E16" s="7">
         <v>211874.01151657099</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F16" s="13">
+        <v>217739.98737335199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17" s="7">
         <v>7708769.7961330405</v>
@@ -808,10 +848,13 @@
       <c r="E17" s="7">
         <v>6592338.6468887301</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F17" s="13">
+        <v>5931237.2560501099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B18" s="7">
         <v>5469833.8876962699</v>
@@ -825,10 +868,13 @@
       <c r="E18" s="7">
         <v>2061818.73893738</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F18" s="13">
+        <v>2537759.55283642</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19" s="7">
         <v>4486859.0157032004</v>
@@ -842,10 +888,13 @@
       <c r="E19" s="7">
         <v>1039342.16594696</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="F19" s="13">
+        <v>1599300.2072572701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" s="7">
         <v>982974.871993065</v>
@@ -859,10 +908,13 @@
       <c r="E20" s="7">
         <v>1022476.57299042</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F20" s="13">
+        <v>938459.34557914699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21" s="7">
         <v>543725.52919387806</v>
@@ -876,10 +928,13 @@
       <c r="E21" s="7">
         <v>420585.72435378999</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F21" s="13">
+        <v>351650.07960796403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B22" s="7">
         <v>9833118.9194917697</v>
@@ -893,10 +948,13 @@
       <c r="E22" s="7">
         <v>7130983.5219383202</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="13">
+        <v>5839786.4613533001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7">
         <v>48306.193709373503</v>
@@ -910,10 +968,13 @@
       <c r="E23" s="7">
         <v>670407.32002258301</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F23" s="13">
+        <v>398464.17689323402</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="7">
         <v>3036549.8045682898</v>
@@ -927,10 +988,13 @@
       <c r="E24" s="7">
         <v>2631032.5012206999</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F24" s="13">
+        <v>2203528.67221832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="7">
         <v>6748262.9212141</v>
@@ -944,10 +1008,13 @@
       <c r="E25" s="7">
         <v>3829543.7006950402</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F25" s="13">
+        <v>3237793.6122417399</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B26" s="9">
         <v>23231908.9746475</v>
@@ -961,82 +1028,8 @@
       <c r="E26" s="9">
         <v>15997014.919281</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7">
-        <v>4501463.2138013802</v>
-      </c>
-      <c r="C28" s="7">
-        <v>4079637.0557546602</v>
-      </c>
-      <c r="D28" s="7">
-        <v>4835575.8819580097</v>
-      </c>
-      <c r="E28" s="7">
-        <v>3654563.1737708999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="10">
-        <v>2450135.0809335699</v>
-      </c>
-      <c r="C29" s="10">
-        <v>3410956.7188024502</v>
-      </c>
-      <c r="D29" s="10">
-        <v>2823151.1969566299</v>
-      </c>
-      <c r="E29" s="10">
-        <v>2235745.1663017301</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="10">
-        <v>67863186.692090705</v>
-      </c>
-      <c r="C30" s="10">
-        <v>41046260.823265001</v>
-      </c>
-      <c r="D30" s="10">
-        <v>41413409.360004403</v>
-      </c>
-      <c r="E30" s="10">
-        <v>33071936.5544797</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="10">
-        <v>59533</v>
-      </c>
-      <c r="C31" s="10">
-        <v>57016</v>
-      </c>
-      <c r="D31" s="10">
-        <v>56888</v>
-      </c>
-      <c r="E31" s="10">
-        <v>60617</v>
+      <c r="F26" s="14">
+        <v>14526523.257613201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>